<commit_message>
Se agrega y corrige crud de usuario, se añade dataset usuarios
</commit_message>
<xml_diff>
--- a/DataSet/Dataset Departamentos.xlsx
+++ b/DataSet/Dataset Departamentos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AFFE7B-D67F-448A-8046-7A15D5654D65}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292FF5BD-A3D8-44E5-B0F2-B754D6CDC468}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31332" yWindow="-312" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30720" yWindow="1488" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>IdDepartamentoPk</t>
-  </si>
-  <si>
     <t>Departamento</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>Bogota</t>
+  </si>
+  <si>
+    <t>IdDepartamento</t>
   </si>
 </sst>
 </file>
@@ -444,9 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -456,10 +454,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -467,7 +465,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -475,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -483,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -491,7 +489,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -499,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -507,7 +505,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -515,7 +513,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -523,7 +521,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -531,7 +529,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -547,7 +545,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -555,7 +553,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -563,7 +561,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -571,7 +569,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -579,7 +577,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -587,7 +585,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -595,7 +593,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -603,7 +601,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -611,7 +609,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -619,7 +617,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -627,7 +625,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -635,7 +633,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -643,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -651,7 +649,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,7 +657,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -667,7 +665,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -675,7 +673,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -683,7 +681,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -691,7 +689,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -699,7 +697,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -707,7 +705,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -715,7 +713,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,10 +721,11 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>